<commit_message>
start of init tests
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -114,7 +114,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,12 +145,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -164,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -177,9 +171,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -489,7 +480,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+      <selection activeCell="AD18" sqref="AD18:AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -745,7 +736,7 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1065,7 +1056,7 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1205,7 +1196,7 @@
       <c r="V9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="W9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="X9" s="2" t="s">
@@ -1652,7 +1643,7 @@
       <c r="K15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="M15" s="5" t="s">
@@ -1886,7 +1877,7 @@
       <c r="I18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -2171,7 +2162,7 @@
       <c r="X21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Y21" s="6" t="s">
+      <c r="Y21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="Z21" s="1">

</xml_diff>

<commit_message>
1st draft of BoardAdjTargetTests finished.  Needs minor editing
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\workspace\ClueGameExp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
@@ -233,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,7 +475,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD18" sqref="AD18:AE18"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>